<commit_message>
Add web interface components and update production scheduling system
- Add Backend API specification documentation
- Implement web interface with stage formatters
- Add verification CSV files for order processing
- Update preprocessing system and machine configurations
- Add improved scheduling HTML templates
- Update Gantt chart visualization
</commit_message>
<xml_diff>
--- a/python_engine/data/input/불가능한 공정 입력값.xlsx
+++ b/python_engine/data/input/불가능한 공정 입력값.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\OneDrive\바탕 화면\생산계획\스케줄링-0828\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\OneDrive\바탕 화면\생산계획\FastAPI_Scheduling_Server\production-scheduling-system\python_engine\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B010E3-0078-4113-B7E7-EF27A5F919C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA16757-9197-4F79-B9D0-7CAA5D625AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="-15810" windowWidth="10890" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="기계" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>기계인덱스</t>
   </si>
@@ -92,22 +92,6 @@
   </si>
   <si>
     <t>공정명</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>호기</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -148,35 +132,12 @@
     <t>C2270</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>기계</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>이름</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -213,13 +174,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -235,13 +189,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -266,14 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -492,50 +438,44 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="3" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="C2" s="5">
+        <v>45792</v>
       </c>
       <c r="D2" s="5">
-        <v>45792</v>
-      </c>
-      <c r="E2" s="5">
         <v>45793</v>
       </c>
     </row>
@@ -570,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -584,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1019332-7585-442C-9C41-EA8502DDB542}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -600,18 +540,18 @@
     </row>
     <row r="2" spans="1:2" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>